<commit_message>
added inflation (short and long)
</commit_message>
<xml_diff>
--- a/data/e5100.xlsx
+++ b/data/e5100.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarikz/Documents/GitHub/julia-lux/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D929508-CAAD-3947-B6F8-1B1138BCF873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76381929-35D4-6746-9802-F0EFA4E54B3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3720" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="0" yWindow="3720" windowWidth="36680" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="e5100" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="AO6" authorId="0" shapeId="0">
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -38,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA6" authorId="0" shapeId="0">
+    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BH6" authorId="0" shapeId="0">
+    <comment ref="BH6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BJ6" authorId="0" shapeId="0">
+    <comment ref="BJ6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BM6" authorId="0" shapeId="0">
+    <comment ref="BM6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="BV11" authorId="0" shapeId="0">
+    <comment ref="BV11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">(-) Valeur manquante par dÈfaut
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BV12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">(-) Valeur manquante par dÈfaut
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BV13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -117,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BV12" authorId="0" shapeId="0">
+    <comment ref="BV14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BV13" authorId="0" shapeId="0">
+    <comment ref="BV15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -145,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BV14" authorId="0" shapeId="0">
+    <comment ref="BV16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -159,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BV15" authorId="0" shapeId="0">
+    <comment ref="BV17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -173,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BV16" authorId="0" shapeId="0">
+    <comment ref="BV18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -187,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BV17" authorId="0" shapeId="0">
+    <comment ref="BV19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -201,35 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BV18" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">(-) Valeur manquante par dÈfaut
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BV19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">(-) Valeur manquante par dÈfaut
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A20" authorId="0" shapeId="0">
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -242,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BV20" authorId="0" shapeId="0">
+    <comment ref="BV20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -254,6 +274,16 @@
           <t xml:space="preserve">(-) Valeur manquante par dÈfaut
 </t>
         </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -269,9 +299,6 @@
     <t>STATEC</t>
   </si>
   <si>
-    <t>AnnÈe</t>
-  </si>
-  <si>
     <t>1948</t>
   </si>
   <si>
@@ -497,18 +524,12 @@
     <t>Janvier</t>
   </si>
   <si>
-    <t>FÈvrier</t>
-  </si>
-  <si>
     <t>Mars</t>
   </si>
   <si>
     <t>Avril</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Mai</t>
   </si>
   <si>
@@ -518,9 +539,6 @@
     <t>Juillet</t>
   </si>
   <si>
-    <t>Ao˚t</t>
-  </si>
-  <si>
     <t>Septembre</t>
   </si>
   <si>
@@ -530,16 +548,28 @@
     <t>Novembre</t>
   </si>
   <si>
-    <t>DÈcembre</t>
-  </si>
-  <si>
     <t>Moyennes annuelles</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>Annee</t>
+  </si>
+  <si>
+    <t>Fevrier</t>
+  </si>
+  <si>
+    <t>Aout</t>
+  </si>
+  <si>
+    <t>Decembre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -887,258 +917,260 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>9</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>10</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>11</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>13</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>14</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>15</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>16</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>18</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>19</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>20</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>21</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>22</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>23</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>24</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>25</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>26</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>27</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>28</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>29</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>30</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>31</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>32</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>33</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>34</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>35</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>36</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>37</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>38</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>39</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>40</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>42</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>43</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AR6" t="s">
         <v>44</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AS6" t="s">
         <v>45</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AT6" t="s">
         <v>46</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AU6" t="s">
         <v>47</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AV6" t="s">
         <v>48</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AW6" t="s">
         <v>49</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AX6" t="s">
         <v>50</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AY6" t="s">
         <v>51</v>
       </c>
-      <c r="AY6" t="s">
+      <c r="AZ6" t="s">
         <v>52</v>
       </c>
-      <c r="AZ6" t="s">
+      <c r="BA6" t="s">
         <v>53</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="BB6" t="s">
         <v>54</v>
       </c>
-      <c r="BB6" t="s">
+      <c r="BC6" t="s">
         <v>55</v>
       </c>
-      <c r="BC6" t="s">
+      <c r="BD6" t="s">
         <v>56</v>
       </c>
-      <c r="BD6" t="s">
+      <c r="BE6" t="s">
         <v>57</v>
       </c>
-      <c r="BE6" t="s">
+      <c r="BF6" t="s">
         <v>58</v>
       </c>
-      <c r="BF6" t="s">
+      <c r="BG6" t="s">
         <v>59</v>
       </c>
-      <c r="BG6" t="s">
+      <c r="BH6" t="s">
         <v>60</v>
       </c>
-      <c r="BH6" t="s">
+      <c r="BI6" t="s">
         <v>61</v>
       </c>
-      <c r="BI6" t="s">
+      <c r="BJ6" t="s">
         <v>62</v>
       </c>
-      <c r="BJ6" t="s">
+      <c r="BK6" t="s">
         <v>63</v>
       </c>
-      <c r="BK6" t="s">
+      <c r="BL6" t="s">
         <v>64</v>
       </c>
-      <c r="BL6" t="s">
+      <c r="BM6" t="s">
         <v>65</v>
       </c>
-      <c r="BM6" t="s">
+      <c r="BN6" t="s">
         <v>66</v>
       </c>
-      <c r="BN6" t="s">
+      <c r="BO6" t="s">
         <v>67</v>
       </c>
-      <c r="BO6" t="s">
+      <c r="BP6" t="s">
         <v>68</v>
       </c>
-      <c r="BP6" t="s">
+      <c r="BQ6" t="s">
         <v>69</v>
       </c>
-      <c r="BQ6" t="s">
+      <c r="BR6" t="s">
         <v>70</v>
       </c>
-      <c r="BR6" t="s">
+      <c r="BS6" t="s">
         <v>71</v>
       </c>
-      <c r="BS6" t="s">
+      <c r="BT6" t="s">
         <v>72</v>
       </c>
-      <c r="BT6" t="s">
+      <c r="BU6" t="s">
         <v>73</v>
       </c>
-      <c r="BU6" t="s">
+      <c r="BV6" t="s">
         <v>74</v>
       </c>
-      <c r="BV6" t="s">
+    </row>
+    <row r="7" spans="1:74" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>77</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -1360,9 +1392,9 @@
         <v>871.5</v>
       </c>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B9">
         <v>100.62</v>
@@ -1584,9 +1616,9 @@
         <v>882.5</v>
       </c>
     </row>
-    <row r="10" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10">
         <v>100.84</v>
@@ -1808,9 +1840,9 @@
         <v>876.79</v>
       </c>
     </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11">
         <v>100.78</v>
@@ -2029,12 +2061,12 @@
         <v>871.33</v>
       </c>
       <c r="BV11" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>100.62</v>
@@ -2253,12 +2285,12 @@
         <v>873.32</v>
       </c>
       <c r="BV12" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B13">
         <v>100.93</v>
@@ -2477,12 +2509,12 @@
         <v>872.74123050000003</v>
       </c>
       <c r="BV13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:74" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:74" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>84</v>
       </c>
       <c r="B14">
         <v>102.18</v>
@@ -2701,12 +2733,12 @@
         <v>866.79</v>
       </c>
       <c r="BV14" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B15">
         <v>102.76</v>
@@ -2925,12 +2957,12 @@
         <v>876.96</v>
       </c>
       <c r="BV15" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B16">
         <v>102.29</v>
@@ -3149,12 +3181,12 @@
         <v>875.63520900000003</v>
       </c>
       <c r="BV16" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B17">
         <v>101.26</v>
@@ -3373,12 +3405,12 @@
         <v>875.55252389999998</v>
       </c>
       <c r="BV17" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B18">
         <v>101.09</v>
@@ -3597,12 +3629,12 @@
         <v>875.88</v>
       </c>
       <c r="BV18" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B19">
         <v>101.13</v>
@@ -3821,12 +3853,12 @@
         <v>877.12</v>
       </c>
       <c r="BV19" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B20">
         <v>101.21</v>
@@ -4045,7 +4077,7 @@
         <v>871.57</v>
       </c>
       <c r="BV20" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>